<commit_message>
Updated files and added data sheets
</commit_message>
<xml_diff>
--- a/BSPD/BSPD BOM.xlsx
+++ b/BSPD/BSPD BOM.xlsx
@@ -1,18 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28702"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raajchatterjee/Personal/Team Phantom/BSPD/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Faraz\Documents\Team Phantom\hardware\BSPD\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9230B1D-EE24-442F-8188-666468F369F5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="200" yWindow="460" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="200" yWindow="460" windowWidth="28800" windowHeight="17600" tabRatio="494" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="BOM" sheetId="1" r:id="rId1"/>
+    <sheet name="PCB (Surface Mount)" sheetId="1" r:id="rId1"/>
+    <sheet name="Prototype (Through Hole)" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="47">
   <si>
     <t xml:space="preserve">Component </t>
   </si>
@@ -41,15 +43,9 @@
     <t>Comparator</t>
   </si>
   <si>
-    <t>http://www.ti.com/product/LM2903/description</t>
-  </si>
-  <si>
     <t>Quantity</t>
   </si>
   <si>
-    <t>TLV3202-Q1</t>
-  </si>
-  <si>
     <t>Channels</t>
   </si>
   <si>
@@ -62,9 +58,6 @@
     <t>AND Gate</t>
   </si>
   <si>
-    <t xml:space="preserve">10 k </t>
-  </si>
-  <si>
     <t>Resistor</t>
   </si>
   <si>
@@ -74,24 +67,6 @@
     <t>50 uF</t>
   </si>
   <si>
-    <t>5.2 k</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 k </t>
-  </si>
-  <si>
-    <t>6 k</t>
-  </si>
-  <si>
-    <t>3.5 k</t>
-  </si>
-  <si>
-    <t>SN74LVC2G08</t>
-  </si>
-  <si>
-    <t>http://www.ti.com/product/SN74LVC2G08</t>
-  </si>
-  <si>
     <t>Package</t>
   </si>
   <si>
@@ -114,13 +89,105 @@
   </si>
   <si>
     <t>C1</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/CMF502K0000BEEB/CMF2.0KQBCT-ND/2197138/?itemSeq=270847147</t>
+  </si>
+  <si>
+    <t>TLV3202AIDGKR‎</t>
+  </si>
+  <si>
+    <t>SN74AHC1G04DCKR‎</t>
+  </si>
+  <si>
+    <t>SN74LVC2G08DCUR‎</t>
+  </si>
+  <si>
+    <t>Inverter</t>
+  </si>
+  <si>
+    <t>U?</t>
+  </si>
+  <si>
+    <t>NDS355AN</t>
+  </si>
+  <si>
+    <t>Transistor</t>
+  </si>
+  <si>
+    <t>Q?</t>
+  </si>
+  <si>
+    <t>SC70-5</t>
+  </si>
+  <si>
+    <t>VSSOP-8</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/texas-instruments/SN74AHC1G04DCKR/296-1090-1-ND/276358</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/texas-instruments/SN74LVC2G08DCUR/296-13264-1-ND/484473</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/texas-instruments/TLV3202AIDGKR/296-39262-1-ND/5143254</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <r>
+      <t>10 k</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Ω</t>
+    </r>
+  </si>
+  <si>
+    <t>5.2 kΩ</t>
+  </si>
+  <si>
+    <t>2 kΩ</t>
+  </si>
+  <si>
+    <t>6 kΩ</t>
+  </si>
+  <si>
+    <t>3.5 kΩ</t>
+  </si>
+  <si>
+    <t>SSOT-3</t>
+  </si>
+  <si>
+    <t>Axial</t>
+  </si>
+  <si>
+    <t>‎LM393N/NOPB‎</t>
+  </si>
+  <si>
+    <t>‎CD4081BE‎</t>
+  </si>
+  <si>
+    <t>SN74HC14N‎</t>
+  </si>
+  <si>
+    <t>PCB</t>
+  </si>
+  <si>
+    <t>Prototype</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -128,16 +195,50 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -145,14 +246,121 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -160,6 +368,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -427,168 +638,386 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="10.6640625" style="5"/>
     <col min="2" max="2" width="24" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="9" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" customWidth="1"/>
-    <col min="6" max="6" width="44.83203125" customWidth="1"/>
-    <col min="7" max="7" width="20.83203125" customWidth="1"/>
+    <col min="4" max="4" width="9" style="5" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="21.25" customWidth="1"/>
+    <col min="7" max="7" width="14.25" style="5" customWidth="1"/>
+    <col min="8" max="8" width="51.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" ht="20.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" t="s">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="10" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="E2">
+      <c r="D2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="5">
         <v>2</v>
       </c>
       <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="5">
+        <v>2</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" s="5">
+        <v>1</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="5">
+        <v>1</v>
+      </c>
+      <c r="F4" s="4"/>
+      <c r="G4" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="5">
+        <v>1</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="5">
+        <v>1</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" s="5">
+        <v>1</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H6" s="7"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" s="5">
+        <v>1</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" s="5">
+        <v>1</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="5">
+        <v>1</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" s="5">
+        <v>1</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" s="5">
+        <v>1</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" s="5">
+        <v>1</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" s="5">
+        <v>1</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="5">
         <v>4</v>
       </c>
-      <c r="G2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3">
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" s="5">
+        <v>1</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B17" s="11"/>
+      <c r="C17" s="13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B18" s="12"/>
+      <c r="C18" s="14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{0897690E-7732-4993-8CB0-2F26D4A83D2C}"/>
+    <hyperlink ref="H8" r:id="rId2" xr:uid="{F1952051-0242-407B-92C8-78601ABB6882}"/>
+    <hyperlink ref="H9" r:id="rId3" xr:uid="{F2EBBAFC-E004-4024-BB3E-C34D1501207D}"/>
+    <hyperlink ref="H4" r:id="rId4" xr:uid="{DB062D3E-9C99-4D1C-A3B2-C2CBF1E84EE9}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1179586F-5AED-43AA-9A03-49592616702C}">
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView zoomScale="115" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="10.33203125" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" customWidth="1"/>
+    <col min="8" max="8" width="15.4140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="20.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>1</v>
-      </c>
-      <c r="B6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>1</v>
-      </c>
-      <c r="B7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>1</v>
-      </c>
-      <c r="B8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>1</v>
-      </c>
-      <c r="B9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated BOM and Schematic
</commit_message>
<xml_diff>
--- a/BSPD/BSPD BOM.xlsx
+++ b/BSPD/BSPD BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Faraz\Documents\Team Phantom\hardware\BSPD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9230B1D-EE24-442F-8188-666468F369F5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23F7D598-8206-479E-9B0F-C22B3C5C882F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="200" yWindow="460" windowWidth="28800" windowHeight="17600" tabRatio="494" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="63">
   <si>
     <t xml:space="preserve">Component </t>
   </si>
@@ -52,9 +52,6 @@
     <t>Features</t>
   </si>
   <si>
-    <t>Hysterisis, Push-pull O/P</t>
-  </si>
-  <si>
     <t>AND Gate</t>
   </si>
   <si>
@@ -64,36 +61,15 @@
     <t>Capacitor</t>
   </si>
   <si>
-    <t>50 uF</t>
-  </si>
-  <si>
     <t>Package</t>
   </si>
   <si>
     <t>Symbol</t>
   </si>
   <si>
-    <t>R1</t>
-  </si>
-  <si>
-    <t>R2</t>
-  </si>
-  <si>
-    <t>R3</t>
-  </si>
-  <si>
-    <t>R4</t>
-  </si>
-  <si>
-    <t>R5</t>
-  </si>
-  <si>
     <t>C1</t>
   </si>
   <si>
-    <t>https://www.digikey.ca/product-detail/en/CMF502K0000BEEB/CMF2.0KQBCT-ND/2197138/?itemSeq=270847147</t>
-  </si>
-  <si>
     <t>TLV3202AIDGKR‎</t>
   </si>
   <si>
@@ -136,38 +112,9 @@
     <t>N/A</t>
   </si>
   <si>
-    <r>
-      <t>10 k</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Ω</t>
-    </r>
-  </si>
-  <si>
-    <t>5.2 kΩ</t>
-  </si>
-  <si>
-    <t>2 kΩ</t>
-  </si>
-  <si>
-    <t>6 kΩ</t>
-  </si>
-  <si>
-    <t>3.5 kΩ</t>
-  </si>
-  <si>
     <t>SSOT-3</t>
   </si>
   <si>
-    <t>Axial</t>
-  </si>
-  <si>
     <t>‎LM393N/NOPB‎</t>
   </si>
   <si>
@@ -177,17 +124,107 @@
     <t>SN74HC14N‎</t>
   </si>
   <si>
-    <t>PCB</t>
-  </si>
-  <si>
-    <t>Prototype</t>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>IC COMPAR PWR RRI DL PP 8VSSOP</t>
+  </si>
+  <si>
+    <t>IC GATE AND 2CH 2-INP US8</t>
+  </si>
+  <si>
+    <t>IC INVERTER 1CH 1-INP SC70-5</t>
+  </si>
+  <si>
+    <t>RES SMD 10K OHM 0.1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>R?</t>
+  </si>
+  <si>
+    <t>RES SMD 3.48K OHM 0.1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>RES SMD 5.23K OHM 0.1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>RES SMD 2K OHM 0.1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>RES SMD 6.04K OHM 0.1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>MOSFET N-CH 30V 1.7A SSOT3</t>
+  </si>
+  <si>
+    <t>0805</t>
+  </si>
+  <si>
+    <t>Web ID:</t>
+  </si>
+  <si>
+    <t>Access ID:</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/ERA-6AEB202V/P2.0KDACT-ND/1465954/?itemSeq=273754536</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/ERA-6AEB103V/P10KDACT-ND/1465971/?itemSeq=273771437</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.ca/product-detail/en/ERA-6AEB5231V/P5.23KDACT-ND/3075171/?itemSeq=273754610 </t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/ERA-6AEB6041V/P6.04KDACT-ND/3075201/?itemSeq=273770790</t>
+  </si>
+  <si>
+    <t>RES SMD 499 OHM 0.1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>CAP ALUM 47UF 10% 10V RADIAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.ca/product-detail/en/NDS355AN/NDS355ANCT-ND/459000/?itemSeq=273772204 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.ca/product-detail/en/ERA-6AEB3481V/P3.48KDACT-ND/3075099/?itemSeq=273754823 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.ca/product-detail/en/ERA-6AEB4990V/P499DACT-ND/3075160/?itemSeq=273771664 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.ca/product-detail/en/UKL1A470KDDANA/493-16841-ND/2598365/?itemSeq=273781180 </t>
+  </si>
+  <si>
+    <t>‎ERA-6AEB202V‎</t>
+  </si>
+  <si>
+    <t>‎ERA-6AEB5231V</t>
+  </si>
+  <si>
+    <t>ERA-6AEB3481V</t>
+  </si>
+  <si>
+    <t>ERA-6AEB6041V</t>
+  </si>
+  <si>
+    <t>ERA-6AEB103V</t>
+  </si>
+  <si>
+    <t>ERA-6AEB4990V</t>
+  </si>
+  <si>
+    <t>UKL1A470KDDANA</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/short/jn22fd</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -204,12 +241,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <u/>
       <sz val="12"/>
       <color theme="10"/>
@@ -218,7 +249,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -231,14 +262,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="8">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -327,12 +352,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -343,21 +386,28 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -639,22 +689,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" style="5"/>
+    <col min="1" max="1" width="10.6640625" style="4"/>
     <col min="2" max="2" width="24" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="9" style="5" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="21.25" customWidth="1"/>
-    <col min="7" max="7" width="14.25" style="5" customWidth="1"/>
-    <col min="8" max="8" width="51.25" customWidth="1"/>
+    <col min="4" max="4" width="31.4140625" customWidth="1"/>
+    <col min="5" max="5" width="9" style="4" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="14.25" style="4" customWidth="1"/>
+    <col min="8" max="8" width="81.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="20.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -668,329 +718,372 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="G1" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="5">
-        <v>1</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>21</v>
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>13</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="4">
+        <v>2</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="5">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="F2" t="s">
+      <c r="B3" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H2" s="6" t="s">
+      <c r="D3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="5">
+      <c r="E3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="G3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" s="4">
+        <v>1</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="4">
+        <v>1</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C3" t="s">
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="4">
+        <v>1</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="4">
+        <v>1</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" s="4">
+        <v>1</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" s="5">
-        <v>2</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="5">
-        <v>1</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" s="5">
-        <v>1</v>
-      </c>
-      <c r="F4" s="4"/>
-      <c r="G4" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="5">
-        <v>1</v>
-      </c>
-      <c r="B5" s="10" t="s">
+      <c r="D6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" s="5">
-        <v>1</v>
-      </c>
-      <c r="G5" s="5" t="s">
+      <c r="G6" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" s="4">
+        <v>1</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" s="4">
+        <v>1</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="4">
+        <v>1</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" s="5">
-        <v>1</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="E9" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" s="4">
+        <v>1</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" s="4">
+        <v>1</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" s="4">
+        <v>1</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="C12" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="H6" s="7"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="5">
-        <v>1</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="C7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" s="5">
-        <v>1</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="C8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="5">
-        <v>1</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="C9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="5">
-        <v>1</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" s="5">
-        <v>1</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="5">
-        <v>1</v>
-      </c>
-      <c r="B13" s="9" t="s">
+      <c r="D12" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G12" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="C13" t="s">
-        <v>3</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E13" s="5">
-        <v>2</v>
-      </c>
-    </row>
+      <c r="H12" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" s="5">
-        <v>1</v>
-      </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="C14" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E14" s="5">
-        <v>4</v>
+      <c r="C14" s="15">
+        <v>286366203</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" s="5">
-        <v>1</v>
-      </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="C15" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E15" s="5">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B17" s="11"/>
-      <c r="C17" s="13" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B18" s="12"/>
-      <c r="C18" s="14" t="s">
-        <v>46</v>
-      </c>
+      <c r="C15" s="19">
+        <v>17553</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B16" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C16" s="17"/>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B18" s="9"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="8"/>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B19" s="11"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="8"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H2" r:id="rId1" xr:uid="{0897690E-7732-4993-8CB0-2F26D4A83D2C}"/>
-    <hyperlink ref="H8" r:id="rId2" xr:uid="{F1952051-0242-407B-92C8-78601ABB6882}"/>
-    <hyperlink ref="H9" r:id="rId3" xr:uid="{F2EBBAFC-E004-4024-BB3E-C34D1501207D}"/>
-    <hyperlink ref="H4" r:id="rId4" xr:uid="{DB062D3E-9C99-4D1C-A3B2-C2CBF1E84EE9}"/>
+    <hyperlink ref="H4" r:id="rId2" xr:uid="{DB062D3E-9C99-4D1C-A3B2-C2CBF1E84EE9}"/>
+    <hyperlink ref="H8" r:id="rId3" xr:uid="{15FCCD6F-93D5-446F-AFEB-2E132E9F5B5A}"/>
+    <hyperlink ref="H7" r:id="rId4" xr:uid="{6A09E3AD-0B58-4373-944C-063B7DA6BD33}"/>
+    <hyperlink ref="H5" r:id="rId5" xr:uid="{8CF07D9D-E85F-4ED9-AACB-F69CE13F7192}"/>
+    <hyperlink ref="H10" r:id="rId6" xr:uid="{913982C2-EBE9-4B77-BCE5-2413A10EACDB}"/>
+    <hyperlink ref="H11" r:id="rId7" xr:uid="{0A81ECD6-198A-4E4F-90E6-3B08981EB717}"/>
+    <hyperlink ref="H12" r:id="rId8" xr:uid="{576CFD58-AA34-4B62-982E-73EF65A43393}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId9"/>
+  <ignoredErrors>
+    <ignoredError sqref="G11:G12 G6:G10" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1179586F-5AED-43AA-9A03-49592616702C}">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView zoomScale="115" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10.33203125" customWidth="1"/>
     <col min="2" max="2" width="15.33203125" customWidth="1"/>
+    <col min="3" max="3" width="11.08203125" customWidth="1"/>
     <col min="8" max="8" width="15.4140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1005,7 +1098,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>5</v>
@@ -1014,11 +1107,65 @@
         <v>6</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>2</v>
       </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="4">
+        <v>2</v>
+      </c>
+      <c r="H2" s="4"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="4">
+        <v>1</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="4">
+        <v>4</v>
+      </c>
+      <c r="H3" s="4"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" s="4">
+        <v>1</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="4">
+        <v>6</v>
+      </c>
+      <c r="H4" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Schematic free of errors/warnings & PCB doc created
</commit_message>
<xml_diff>
--- a/BSPD/BSPD BOM.xlsx
+++ b/BSPD/BSPD BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Faraz\Documents\Team Phantom\hardware\BSPD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF05FBF0-37A3-48AE-A286-1A9DF7FC0CEC}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0871AA1F-944A-429E-9150-D64D643B1EF3}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="200" yWindow="460" windowWidth="28800" windowHeight="17600" tabRatio="494" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="70">
   <si>
     <t xml:space="preserve">Component </t>
   </si>
@@ -218,6 +218,27 @@
   </si>
   <si>
     <t>https://www.digikey.ca/product-detail/en/CL21A106KPFNNNG/1276-6456-1-ND/5958084/?itemSeq=274494946</t>
+  </si>
+  <si>
+    <t>0436500200‎</t>
+  </si>
+  <si>
+    <t>Connector</t>
+  </si>
+  <si>
+    <t>CONN HEADER 2POS 3MM RT ANG TIN</t>
+  </si>
+  <si>
+    <t>0436500400‎</t>
+  </si>
+  <si>
+    <t>CONN HEADER 4POS 3MM RT ANG TIN</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/0436500400/WM1862-ND/268991/?itemSeq=276688085</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/0436500200/WM1860-ND/268989/?itemSeq=276688088</t>
   </si>
 </sst>
 </file>
@@ -686,10 +707,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -697,7 +718,7 @@
     <col min="1" max="1" width="10.6640625" style="4"/>
     <col min="2" max="2" width="24" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="31.4140625" customWidth="1"/>
+    <col min="4" max="4" width="32.5" customWidth="1"/>
     <col min="5" max="5" width="9" style="4" customWidth="1"/>
     <col min="6" max="6" width="14.33203125" style="4" customWidth="1"/>
     <col min="7" max="7" width="14.25" style="4" customWidth="1"/>
@@ -1016,38 +1037,85 @@
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" s="4">
+        <v>1</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C13" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" t="s">
+        <v>67</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G13" s="12"/>
+      <c r="H13" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B14" s="13" t="s">
+      <c r="A14" s="4">
+        <v>1</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" t="s">
+        <v>64</v>
+      </c>
+      <c r="D14" t="s">
+        <v>65</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G14" s="12"/>
+      <c r="H14" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B15" s="11"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="5"/>
+    </row>
+    <row r="16" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B17" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="C14" s="14">
+      <c r="C17" s="14">
         <v>286621267</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B15" s="17" t="s">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B18" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="18">
+      <c r="C18" s="18">
         <v>42986</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B16" s="15" t="s">
+    <row r="19" spans="2:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B19" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="C16" s="16"/>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B18" s="8"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="7"/>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B19" s="10"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="7"/>
+      <c r="C19" s="16"/>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B21" s="8"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="7"/>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B22" s="10"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
added mounting holes and fixed some design rule errors
</commit_message>
<xml_diff>
--- a/BSPD/BSPD BOM.xlsx
+++ b/BSPD/BSPD BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Faraz\Documents\Team Phantom\hardware\BSPD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0871AA1F-944A-429E-9150-D64D643B1EF3}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44A88220-AE3A-4CC3-BBE6-F3A6A5D0BCB9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="200" yWindow="460" windowWidth="28800" windowHeight="17600" tabRatio="494" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,10 +16,16 @@
     <sheet name="PCB (Surface Mount)" sheetId="1" r:id="rId1"/>
     <sheet name="Prototype (Through Hole)" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -28,8 +34,70 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Faraz</author>
+  </authors>
+  <commentList>
+    <comment ref="B11" authorId="0" shapeId="0" xr:uid="{93C4BE8C-933C-4AF3-B900-C1EFD18900C5}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Faraz:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Jan 6, 2019:
+-currently on backorder from digikey
+-use 15microFarad Cap W/ 33.3kOhm Res</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B12" authorId="0" shapeId="0" xr:uid="{0937F2BA-6C8B-416E-8FA9-4A3DF56D6DF8}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Faraz:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Jan 6, 2019:
+-currently on backorder from digikey
+-use 15microFarad Cap W/ 33.3kOhm Res</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="83">
   <si>
     <t xml:space="preserve">Component </t>
   </si>
@@ -82,9 +150,6 @@
     <t>U?</t>
   </si>
   <si>
-    <t>NDS355AN</t>
-  </si>
-  <si>
     <t>Transistor</t>
   </si>
   <si>
@@ -109,9 +174,6 @@
     <t>N/A</t>
   </si>
   <si>
-    <t>SSOT-3</t>
-  </si>
-  <si>
     <t>‎LM393N/NOPB‎</t>
   </si>
   <si>
@@ -148,9 +210,6 @@
     <t>RES SMD 6.04K OHM 0.1% 1/8W 0805</t>
   </si>
   <si>
-    <t>MOSFET N-CH 30V 1.7A SSOT3</t>
-  </si>
-  <si>
     <t>0805</t>
   </si>
   <si>
@@ -172,9 +231,6 @@
     <t>RES SMD 499 OHM 0.1% 1/8W 0805</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.digikey.ca/product-detail/en/NDS355AN/NDS355ANCT-ND/459000/?itemSeq=273772204 </t>
-  </si>
-  <si>
     <t xml:space="preserve">https://www.digikey.ca/product-detail/en/ERA-6AEB3481V/P3.48KDACT-ND/3075099/?itemSeq=273754823 </t>
   </si>
   <si>
@@ -239,13 +295,64 @@
   </si>
   <si>
     <t>https://www.digikey.ca/product-detail/en/0436500200/WM1860-ND/268989/?itemSeq=276688088</t>
+  </si>
+  <si>
+    <t>CAP CER 33UF 10V X5R 0805</t>
+  </si>
+  <si>
+    <t>‎43030-0001‎</t>
+  </si>
+  <si>
+    <t>Connector Receptacle</t>
+  </si>
+  <si>
+    <t>CONN TERM FEMALE 20-24AWG TIN</t>
+  </si>
+  <si>
+    <t>C2012X5R1A336M125AC‎</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/C2012X5R1A336M125AC/445-8238-1-ND/2812080/?itemSeq=281051761</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/43030-0001/WM1837CT-ND/467810/?itemSeq=281050768</t>
+  </si>
+  <si>
+    <t>Tau (sec)</t>
+  </si>
+  <si>
+    <t>R (Ohm)</t>
+  </si>
+  <si>
+    <t>C (F)</t>
+  </si>
+  <si>
+    <t>‎ERA-6AEB153V‎</t>
+  </si>
+  <si>
+    <t>RES SMD 15K OHM 0.1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/ERA-6AEB153V/P15KDACT-ND/1465975/?itemSeq=281051755</t>
+  </si>
+  <si>
+    <t>MOSFET N-CH 50V 200MA SOT-23</t>
+  </si>
+  <si>
+    <t>SOT-23-3</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/BSS138LT3G/BSS138LT3GOSCT-ND/2120566/?itemSeq=274498102</t>
+  </si>
+  <si>
+    <t>BSS138LT3G</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -269,8 +376,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -283,8 +409,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -391,12 +523,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -412,10 +562,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -426,6 +572,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -706,11 +879,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -736,7 +909,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>11</v>
@@ -753,16 +926,16 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="4">
-        <v>1</v>
-      </c>
-      <c r="B2" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>12</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>16</v>
@@ -771,24 +944,24 @@
         <v>2</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="7" t="s">
         <v>14</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>16</v>
@@ -797,24 +970,24 @@
         <v>2</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="4">
-        <v>1</v>
-      </c>
-      <c r="B4" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C4" t="s">
         <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>16</v>
@@ -823,299 +996,408 @@
         <v>1</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="4">
-        <v>1</v>
-      </c>
-      <c r="B5" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C5" t="s">
         <v>17</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
+        <v>79</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>18</v>
-      </c>
-      <c r="D5" t="s">
-        <v>39</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>19</v>
       </c>
       <c r="F5" s="4">
         <v>1</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>26</v>
+        <v>80</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>47</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="4">
-        <v>1</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>51</v>
+        <v>2</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>47</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>40</v>
+        <v>24</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>37</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="4">
-        <v>1</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>50</v>
+        <v>2</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>46</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
       </c>
       <c r="D7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G7" s="12" t="s">
+      <c r="H7" s="5" t="s">
         <v>40</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="4">
-        <v>1</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>53</v>
+        <v>2</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>49</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>40</v>
+        <v>24</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>37</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="4">
-        <v>1</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>52</v>
+        <v>2</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>48</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G9" s="12" t="s">
-        <v>40</v>
+        <v>24</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>37</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="4">
-        <v>1</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>54</v>
+        <v>2</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>50</v>
       </c>
       <c r="C10" t="s">
         <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G10" s="12" t="s">
-        <v>40</v>
+        <v>24</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>37</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="4">
-        <v>1</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="C11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="D11" t="s">
-        <v>57</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G11" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>58</v>
+      <c r="D11" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="H11" s="18" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="4">
-        <v>1</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="C12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="D12" t="s">
-        <v>60</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G12" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>62</v>
+      <c r="D12" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="F12" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="H12" s="18" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="4">
-        <v>1</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>66</v>
+        <v>2</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>62</v>
       </c>
       <c r="C13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" t="s">
+        <v>63</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H13" s="5" t="s">
         <v>64</v>
-      </c>
-      <c r="D13" t="s">
-        <v>67</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G13" s="12"/>
-      <c r="H13" s="5" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="4">
-        <v>1</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>63</v>
+        <v>2</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>59</v>
       </c>
       <c r="C14" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D14" t="s">
+        <v>61</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H14" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="F14" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G14" s="12"/>
-      <c r="H14" s="5" t="s">
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" s="4">
+        <v>12</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C15" t="s">
+        <v>68</v>
+      </c>
+      <c r="D15" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B15" s="11"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="5"/>
-    </row>
-    <row r="16" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B17" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="C17" s="14">
+      <c r="E15" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" s="4">
+        <v>2</v>
+      </c>
+      <c r="B16" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" t="s">
+        <v>66</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17" s="4">
+        <v>2</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" t="s">
+        <v>77</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H18" s="5"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B19" s="7"/>
+      <c r="H19" s="5"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B20" s="7"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="5"/>
+    </row>
+    <row r="21" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B22" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" s="10">
         <v>286621267</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B18" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="C18" s="18">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B23" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23" s="14">
         <v>42986</v>
       </c>
     </row>
-    <row r="19" spans="2:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B19" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="C19" s="16"/>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B21" s="8"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="7"/>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B22" s="10"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="7"/>
+    <row r="24" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B24" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" s="12"/>
+    </row>
+    <row r="25" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B26" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="C26" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="D26" s="22" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B27" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="C27" s="24">
+        <f>($B$27/$D$27)</f>
+        <v>33333.333333333336</v>
+      </c>
+      <c r="D27" s="25">
+        <v>1.5E-5</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1123,15 +1405,15 @@
     <hyperlink ref="H4" r:id="rId2" xr:uid="{DB062D3E-9C99-4D1C-A3B2-C2CBF1E84EE9}"/>
     <hyperlink ref="H7" r:id="rId3" xr:uid="{15FCCD6F-93D5-446F-AFEB-2E132E9F5B5A}"/>
     <hyperlink ref="H6" r:id="rId4" xr:uid="{6A09E3AD-0B58-4373-944C-063B7DA6BD33}"/>
-    <hyperlink ref="H5" r:id="rId5" xr:uid="{8CF07D9D-E85F-4ED9-AACB-F69CE13F7192}"/>
-    <hyperlink ref="H9" r:id="rId6" xr:uid="{913982C2-EBE9-4B77-BCE5-2413A10EACDB}"/>
-    <hyperlink ref="H10" r:id="rId7" xr:uid="{0A81ECD6-198A-4E4F-90E6-3B08981EB717}"/>
+    <hyperlink ref="H9" r:id="rId5" xr:uid="{913982C2-EBE9-4B77-BCE5-2413A10EACDB}"/>
+    <hyperlink ref="H10" r:id="rId6" xr:uid="{0A81ECD6-198A-4E4F-90E6-3B08981EB717}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId8"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
   <ignoredErrors>
-    <ignoredError sqref="G10 G6:G9 G12 G11" numberStoredAsText="1"/>
+    <ignoredError sqref="G10 G6:G9 G12 G11 G16:G17" numberStoredAsText="1"/>
   </ignoredErrors>
+  <legacyDrawing r:id="rId8"/>
 </worksheet>
 </file>
 
@@ -1181,8 +1463,8 @@
       <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="11" t="s">
-        <v>27</v>
+      <c r="B2" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -1199,8 +1481,8 @@
       <c r="A3" s="4">
         <v>1</v>
       </c>
-      <c r="B3" s="11" t="s">
-        <v>28</v>
+      <c r="B3" s="7" t="s">
+        <v>26</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
@@ -1217,8 +1499,8 @@
       <c r="A4" s="4">
         <v>1</v>
       </c>
-      <c r="B4" s="11" t="s">
-        <v>29</v>
+      <c r="B4" s="7" t="s">
+        <v>27</v>
       </c>
       <c r="C4" t="s">
         <v>15</v>

</xml_diff>